<commit_message>
Try to add new row
</commit_message>
<xml_diff>
--- a/Examples/Database.xlsx
+++ b/Examples/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Solutions\my-openxml-practice\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10260C0-E6A7-4C53-ABE5-8A22C5E17DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDF7A02-8A5B-4F63-9446-7CEDF3000F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="45972" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -36,7 +36,7 @@
     <x:t>Oleg</x:t>
   </x:si>
   <x:si>
-    <x:t>???</x:t>
+    <x:t>Marina</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:dimension ref="A1:B2"/>
+  <x:dimension ref="A1:B3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C5" sqref="C5"/>
+      <x:selection activeCell="B7" sqref="B7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -385,6 +385,14 @@
         <x:v>Here</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" t="str">
+        <x:v>Elswere</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>

</xml_diff>